<commit_message>
Wrote text and created result charts
Copied zim text into latex as well as reports from wandb
finished Results chapter
Created text for all chapters, still needs second opinion
</commit_message>
<xml_diff>
--- a/code/Vision/Datasets/labels/labels5.xlsx
+++ b/code/Vision/Datasets/labels/labels5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsdepauw/Documents/Lars.nosync/Documents/School/1Ma ing/Masterproef/TWI/code/Vision/Datasets/labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BBE452-D2CA-534C-AEB6-018C31F3CC73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AF20F0-B69E-4A43-9A45-B9DE222F5155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="-17560" windowWidth="26840" windowHeight="15940" xr2:uid="{7C2D2E37-B908-3941-8EC8-7D93A5E6F16B}"/>
+    <workbookView xWindow="11640" yWindow="-20400" windowWidth="26840" windowHeight="15940" xr2:uid="{7C2D2E37-B908-3941-8EC8-7D93A5E6F16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="376">
   <si>
     <t>bullet</t>
   </si>
@@ -351,468 +351,6 @@
   </si>
   <si>
     <t>pn</t>
-  </si>
-  <si>
-    <t>358.0</t>
-  </si>
-  <si>
-    <t>254.0</t>
-  </si>
-  <si>
-    <t>180.0</t>
-  </si>
-  <si>
-    <t>190.0</t>
-  </si>
-  <si>
-    <t>452.0</t>
-  </si>
-  <si>
-    <t>499.0</t>
-  </si>
-  <si>
-    <t>572.0</t>
-  </si>
-  <si>
-    <t>236.0</t>
-  </si>
-  <si>
-    <t>150.0</t>
-  </si>
-  <si>
-    <t>244.0</t>
-  </si>
-  <si>
-    <t>570.0</t>
-  </si>
-  <si>
-    <t>815.0</t>
-  </si>
-  <si>
-    <t>577.0</t>
-  </si>
-  <si>
-    <t>477.0</t>
-  </si>
-  <si>
-    <t>298.0</t>
-  </si>
-  <si>
-    <t>219.0</t>
-  </si>
-  <si>
-    <t>169.0</t>
-  </si>
-  <si>
-    <t>48.0</t>
-  </si>
-  <si>
-    <t>309.0</t>
-  </si>
-  <si>
-    <t>283.0</t>
-  </si>
-  <si>
-    <t>260.0</t>
-  </si>
-  <si>
-    <t>205.0</t>
-  </si>
-  <si>
-    <t>98.0</t>
-  </si>
-  <si>
-    <t>57.0</t>
-  </si>
-  <si>
-    <t>238.0</t>
-  </si>
-  <si>
-    <t>137.0</t>
-  </si>
-  <si>
-    <t>285.0</t>
-  </si>
-  <si>
-    <t>281.0</t>
-  </si>
-  <si>
-    <t>251.0</t>
-  </si>
-  <si>
-    <t>154.0</t>
-  </si>
-  <si>
-    <t>136.0</t>
-  </si>
-  <si>
-    <t>215.0</t>
-  </si>
-  <si>
-    <t>183.0</t>
-  </si>
-  <si>
-    <t>157.0</t>
-  </si>
-  <si>
-    <t>122.0</t>
-  </si>
-  <si>
-    <t>322.0</t>
-  </si>
-  <si>
-    <t>224.0</t>
-  </si>
-  <si>
-    <t>162.0</t>
-  </si>
-  <si>
-    <t>172.0</t>
-  </si>
-  <si>
-    <t>193.0</t>
-  </si>
-  <si>
-    <t>189.0</t>
-  </si>
-  <si>
-    <t>208.0</t>
-  </si>
-  <si>
-    <t>196.0</t>
-  </si>
-  <si>
-    <t>194.0</t>
-  </si>
-  <si>
-    <t>326.0</t>
-  </si>
-  <si>
-    <t>222.0</t>
-  </si>
-  <si>
-    <t>230.0</t>
-  </si>
-  <si>
-    <t>155.0</t>
-  </si>
-  <si>
-    <t>188.0</t>
-  </si>
-  <si>
-    <t>227.0</t>
-  </si>
-  <si>
-    <t>181.0</t>
-  </si>
-  <si>
-    <t>200.0</t>
-  </si>
-  <si>
-    <t>168.0</t>
-  </si>
-  <si>
-    <t>259.0</t>
-  </si>
-  <si>
-    <t>581.0</t>
-  </si>
-  <si>
-    <t>650.0</t>
-  </si>
-  <si>
-    <t>635.0</t>
-  </si>
-  <si>
-    <t>555.0</t>
-  </si>
-  <si>
-    <t>307.0</t>
-  </si>
-  <si>
-    <t>99.0</t>
-  </si>
-  <si>
-    <t>86.0</t>
-  </si>
-  <si>
-    <t>475.0</t>
-  </si>
-  <si>
-    <t>438.0</t>
-  </si>
-  <si>
-    <t>255.0</t>
-  </si>
-  <si>
-    <t>214.0</t>
-  </si>
-  <si>
-    <t>603.0</t>
-  </si>
-  <si>
-    <t>751.0</t>
-  </si>
-  <si>
-    <t>225.0</t>
-  </si>
-  <si>
-    <t>369.0</t>
-  </si>
-  <si>
-    <t>526.0</t>
-  </si>
-  <si>
-    <t>469.0</t>
-  </si>
-  <si>
-    <t>84.0</t>
-  </si>
-  <si>
-    <t>508.0</t>
-  </si>
-  <si>
-    <t>362.0</t>
-  </si>
-  <si>
-    <t>151.0</t>
-  </si>
-  <si>
-    <t>522.0</t>
-  </si>
-  <si>
-    <t>272.0</t>
-  </si>
-  <si>
-    <t>780.0</t>
-  </si>
-  <si>
-    <t>843.0</t>
-  </si>
-  <si>
-    <t>638.0</t>
-  </si>
-  <si>
-    <t>705.0</t>
-  </si>
-  <si>
-    <t>425.0</t>
-  </si>
-  <si>
-    <t>558.0</t>
-  </si>
-  <si>
-    <t>250.0</t>
-  </si>
-  <si>
-    <t>264.0</t>
-  </si>
-  <si>
-    <t>643.0</t>
-  </si>
-  <si>
-    <t>790.0</t>
-  </si>
-  <si>
-    <t>811.0</t>
-  </si>
-  <si>
-    <t>546.0</t>
-  </si>
-  <si>
-    <t>632.0</t>
-  </si>
-  <si>
-    <t>275.0</t>
-  </si>
-  <si>
-    <t>228.0</t>
-  </si>
-  <si>
-    <t>292.0</t>
-  </si>
-  <si>
-    <t>167.0</t>
-  </si>
-  <si>
-    <t>351.0</t>
-  </si>
-  <si>
-    <t>211.0</t>
-  </si>
-  <si>
-    <t>132.0</t>
-  </si>
-  <si>
-    <t>147.0</t>
-  </si>
-  <si>
-    <t>152.0</t>
-  </si>
-  <si>
-    <t>269.0</t>
-  </si>
-  <si>
-    <t>257.0</t>
-  </si>
-  <si>
-    <t>104.0</t>
-  </si>
-  <si>
-    <t>805.0</t>
-  </si>
-  <si>
-    <t>645.0</t>
-  </si>
-  <si>
-    <t>334.0</t>
-  </si>
-  <si>
-    <t>246.0</t>
-  </si>
-  <si>
-    <t>530.0</t>
-  </si>
-  <si>
-    <t>505.0</t>
-  </si>
-  <si>
-    <t>450.0</t>
-  </si>
-  <si>
-    <t>525.0</t>
-  </si>
-  <si>
-    <t>433.0</t>
-  </si>
-  <si>
-    <t>403.0</t>
-  </si>
-  <si>
-    <t>590.0</t>
-  </si>
-  <si>
-    <t>538.0</t>
-  </si>
-  <si>
-    <t>532.0</t>
-  </si>
-  <si>
-    <t>368.0</t>
-  </si>
-  <si>
-    <t>722.0</t>
-  </si>
-  <si>
-    <t>481.0</t>
-  </si>
-  <si>
-    <t>566.0</t>
-  </si>
-  <si>
-    <t>759.0</t>
-  </si>
-  <si>
-    <t>337.0</t>
-  </si>
-  <si>
-    <t>402.0</t>
-  </si>
-  <si>
-    <t>536.0</t>
-  </si>
-  <si>
-    <t>485.0</t>
-  </si>
-  <si>
-    <t>494.0</t>
-  </si>
-  <si>
-    <t>451.0</t>
-  </si>
-  <si>
-    <t>289.0</t>
-  </si>
-  <si>
-    <t>456.0</t>
-  </si>
-  <si>
-    <t>177.0</t>
-  </si>
-  <si>
-    <t>133.0</t>
-  </si>
-  <si>
-    <t>213.0</t>
-  </si>
-  <si>
-    <t>423.0</t>
-  </si>
-  <si>
-    <t>626.0</t>
-  </si>
-  <si>
-    <t>627.0</t>
-  </si>
-  <si>
-    <t>757.0</t>
-  </si>
-  <si>
-    <t>287.0</t>
-  </si>
-  <si>
-    <t>615.0</t>
-  </si>
-  <si>
-    <t>458.0</t>
-  </si>
-  <si>
-    <t>301.0</t>
-  </si>
-  <si>
-    <t>297.0</t>
-  </si>
-  <si>
-    <t>245.0</t>
-  </si>
-  <si>
-    <t>204.0</t>
-  </si>
-  <si>
-    <t>414.0</t>
-  </si>
-  <si>
-    <t>390.0</t>
-  </si>
-  <si>
-    <t>430.0</t>
-  </si>
-  <si>
-    <t>527.0</t>
-  </si>
-  <si>
-    <t>372.0</t>
-  </si>
-  <si>
-    <t>459.0</t>
-  </si>
-  <si>
-    <t>373.0</t>
-  </si>
-  <si>
-    <t>486.0</t>
-  </si>
-  <si>
-    <t>173.0</t>
-  </si>
-  <si>
-    <t>359.0</t>
-  </si>
-  <si>
-    <t>321.0</t>
-  </si>
-  <si>
-    <t>335.0</t>
   </si>
   <si>
     <t>batch_011_plate_001</t>
@@ -1988,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{152B82BB-6E99-EB4E-9EF9-F54D5CEADF20}">
   <dimension ref="A1:F281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="E186" sqref="E186"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4033,13 +3571,13 @@
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>260</v>
+        <v>106</v>
       </c>
       <c r="E102" t="s">
-        <v>261</v>
-      </c>
-      <c r="F102" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="F102">
+        <v>358</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -4053,13 +3591,13 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>260</v>
+        <v>106</v>
       </c>
       <c r="E103" t="s">
-        <v>262</v>
-      </c>
-      <c r="F103" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="F103">
+        <v>254</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -4073,13 +3611,13 @@
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
       <c r="E104" t="s">
-        <v>264</v>
-      </c>
-      <c r="F104" t="s">
-        <v>108</v>
+        <v>110</v>
+      </c>
+      <c r="F104">
+        <v>180</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -4093,13 +3631,13 @@
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
       <c r="E105" t="s">
-        <v>265</v>
-      </c>
-      <c r="F105" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="F105">
+        <v>190</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -4113,13 +3651,13 @@
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>266</v>
+        <v>112</v>
       </c>
       <c r="E106" t="s">
-        <v>267</v>
-      </c>
-      <c r="F106" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="F106">
+        <v>452</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -4133,13 +3671,13 @@
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>266</v>
+        <v>112</v>
       </c>
       <c r="E107" t="s">
-        <v>268</v>
-      </c>
-      <c r="F107" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="F107">
+        <v>499</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -4153,13 +3691,13 @@
         <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>269</v>
+        <v>115</v>
       </c>
       <c r="E108" t="s">
-        <v>270</v>
-      </c>
-      <c r="F108" t="s">
-        <v>112</v>
+        <v>116</v>
+      </c>
+      <c r="F108">
+        <v>572</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -4173,13 +3711,13 @@
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>269</v>
+        <v>115</v>
       </c>
       <c r="E109" t="s">
-        <v>271</v>
-      </c>
-      <c r="F109" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="F109">
+        <v>236</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -4193,13 +3731,13 @@
         <v>0</v>
       </c>
       <c r="D110" t="s">
-        <v>272</v>
+        <v>118</v>
       </c>
       <c r="E110" t="s">
-        <v>273</v>
-      </c>
-      <c r="F110" t="s">
-        <v>114</v>
+        <v>119</v>
+      </c>
+      <c r="F110">
+        <v>150</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -4213,13 +3751,13 @@
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>272</v>
+        <v>118</v>
       </c>
       <c r="E111" t="s">
-        <v>274</v>
-      </c>
-      <c r="F111" t="s">
-        <v>115</v>
+        <v>120</v>
+      </c>
+      <c r="F111">
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -4233,13 +3771,13 @@
         <v>0</v>
       </c>
       <c r="D112" t="s">
-        <v>275</v>
+        <v>121</v>
       </c>
       <c r="E112" t="s">
-        <v>276</v>
-      </c>
-      <c r="F112" t="s">
-        <v>116</v>
+        <v>122</v>
+      </c>
+      <c r="F112">
+        <v>570</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -4253,13 +3791,13 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>275</v>
+        <v>121</v>
       </c>
       <c r="E113" t="s">
-        <v>277</v>
-      </c>
-      <c r="F113" t="s">
-        <v>117</v>
+        <v>123</v>
+      </c>
+      <c r="F113">
+        <v>815</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -4273,13 +3811,13 @@
         <v>0</v>
       </c>
       <c r="D114" t="s">
-        <v>278</v>
+        <v>124</v>
       </c>
       <c r="E114" t="s">
-        <v>279</v>
-      </c>
-      <c r="F114" t="s">
-        <v>118</v>
+        <v>125</v>
+      </c>
+      <c r="F114">
+        <v>577</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -4293,13 +3831,13 @@
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>278</v>
+        <v>124</v>
       </c>
       <c r="E115" t="s">
-        <v>280</v>
-      </c>
-      <c r="F115" t="s">
-        <v>119</v>
+        <v>126</v>
+      </c>
+      <c r="F115">
+        <v>477</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -4313,13 +3851,13 @@
         <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>281</v>
+        <v>127</v>
       </c>
       <c r="E116" t="s">
-        <v>282</v>
-      </c>
-      <c r="F116" t="s">
-        <v>120</v>
+        <v>128</v>
+      </c>
+      <c r="F116">
+        <v>298</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -4333,13 +3871,13 @@
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>281</v>
+        <v>127</v>
       </c>
       <c r="E117" t="s">
-        <v>283</v>
-      </c>
-      <c r="F117" t="s">
-        <v>121</v>
+        <v>129</v>
+      </c>
+      <c r="F117">
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -4353,13 +3891,13 @@
         <v>0</v>
       </c>
       <c r="D118" t="s">
-        <v>284</v>
+        <v>130</v>
       </c>
       <c r="E118" t="s">
-        <v>285</v>
-      </c>
-      <c r="F118" t="s">
-        <v>109</v>
+        <v>131</v>
+      </c>
+      <c r="F118">
+        <v>190</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -4373,13 +3911,13 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>284</v>
+        <v>130</v>
       </c>
       <c r="E119" t="s">
-        <v>286</v>
-      </c>
-      <c r="F119" t="s">
-        <v>122</v>
+        <v>132</v>
+      </c>
+      <c r="F119">
+        <v>169</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -4393,13 +3931,13 @@
         <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>287</v>
+        <v>133</v>
       </c>
       <c r="E120" t="s">
-        <v>288</v>
-      </c>
-      <c r="F120" t="s">
-        <v>123</v>
+        <v>134</v>
+      </c>
+      <c r="F120">
+        <v>48</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -4413,13 +3951,13 @@
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>287</v>
+        <v>133</v>
       </c>
       <c r="E121" t="s">
-        <v>289</v>
-      </c>
-      <c r="F121" t="s">
-        <v>124</v>
+        <v>135</v>
+      </c>
+      <c r="F121">
+        <v>309</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -4433,13 +3971,13 @@
         <v>0</v>
       </c>
       <c r="D122" t="s">
-        <v>290</v>
+        <v>136</v>
       </c>
       <c r="E122" t="s">
-        <v>291</v>
-      </c>
-      <c r="F122" t="s">
-        <v>125</v>
+        <v>137</v>
+      </c>
+      <c r="F122">
+        <v>283</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -4453,13 +3991,13 @@
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>290</v>
+        <v>136</v>
       </c>
       <c r="E123" t="s">
-        <v>292</v>
-      </c>
-      <c r="F123" t="s">
-        <v>126</v>
+        <v>138</v>
+      </c>
+      <c r="F123">
+        <v>260</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -4473,13 +4011,13 @@
         <v>0</v>
       </c>
       <c r="D124" t="s">
-        <v>293</v>
+        <v>139</v>
       </c>
       <c r="E124" t="s">
-        <v>294</v>
-      </c>
-      <c r="F124" t="s">
-        <v>109</v>
+        <v>140</v>
+      </c>
+      <c r="F124">
+        <v>190</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -4493,13 +4031,13 @@
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>293</v>
+        <v>139</v>
       </c>
       <c r="E125" t="s">
-        <v>295</v>
-      </c>
-      <c r="F125" t="s">
-        <v>127</v>
+        <v>141</v>
+      </c>
+      <c r="F125">
+        <v>205</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -4513,13 +4051,13 @@
         <v>0</v>
       </c>
       <c r="D126" t="s">
-        <v>296</v>
+        <v>142</v>
       </c>
       <c r="E126" t="s">
-        <v>297</v>
-      </c>
-      <c r="F126" t="s">
-        <v>128</v>
+        <v>143</v>
+      </c>
+      <c r="F126">
+        <v>98</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -4533,13 +4071,13 @@
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>296</v>
+        <v>142</v>
       </c>
       <c r="E127" t="s">
-        <v>298</v>
-      </c>
-      <c r="F127" t="s">
-        <v>129</v>
+        <v>144</v>
+      </c>
+      <c r="F127">
+        <v>57</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -4553,13 +4091,13 @@
         <v>0</v>
       </c>
       <c r="D128" t="s">
-        <v>299</v>
+        <v>145</v>
       </c>
       <c r="E128" t="s">
-        <v>300</v>
-      </c>
-      <c r="F128" t="s">
-        <v>130</v>
+        <v>146</v>
+      </c>
+      <c r="F128">
+        <v>238</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -4573,13 +4111,13 @@
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>299</v>
+        <v>145</v>
       </c>
       <c r="E129" t="s">
-        <v>301</v>
-      </c>
-      <c r="F129" t="s">
-        <v>131</v>
+        <v>147</v>
+      </c>
+      <c r="F129">
+        <v>137</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -4593,13 +4131,13 @@
         <v>0</v>
       </c>
       <c r="D130" t="s">
-        <v>302</v>
+        <v>148</v>
       </c>
       <c r="E130" t="s">
-        <v>303</v>
-      </c>
-      <c r="F130" t="s">
-        <v>132</v>
+        <v>149</v>
+      </c>
+      <c r="F130">
+        <v>285</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -4613,13 +4151,13 @@
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>302</v>
+        <v>148</v>
       </c>
       <c r="E131" t="s">
-        <v>304</v>
-      </c>
-      <c r="F131" t="s">
-        <v>133</v>
+        <v>150</v>
+      </c>
+      <c r="F131">
+        <v>281</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -4633,13 +4171,13 @@
         <v>0</v>
       </c>
       <c r="D132" t="s">
-        <v>305</v>
+        <v>151</v>
       </c>
       <c r="E132" t="s">
-        <v>306</v>
-      </c>
-      <c r="F132" t="s">
-        <v>134</v>
+        <v>152</v>
+      </c>
+      <c r="F132">
+        <v>251</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
@@ -4653,13 +4191,13 @@
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>305</v>
+        <v>151</v>
       </c>
       <c r="E133" t="s">
-        <v>307</v>
-      </c>
-      <c r="F133" t="s">
-        <v>135</v>
+        <v>153</v>
+      </c>
+      <c r="F133">
+        <v>154</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -4673,12 +4211,12 @@
         <v>0</v>
       </c>
       <c r="D134" t="s">
-        <v>308</v>
+        <v>154</v>
       </c>
       <c r="E134" t="s">
-        <v>309</v>
-      </c>
-      <c r="F134" t="s">
+        <v>155</v>
+      </c>
+      <c r="F134">
         <v>136</v>
       </c>
     </row>
@@ -4693,13 +4231,13 @@
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>308</v>
+        <v>154</v>
       </c>
       <c r="E135" t="s">
-        <v>310</v>
-      </c>
-      <c r="F135" t="s">
-        <v>137</v>
+        <v>156</v>
+      </c>
+      <c r="F135">
+        <v>215</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -4713,13 +4251,13 @@
         <v>0</v>
       </c>
       <c r="D136" t="s">
-        <v>311</v>
+        <v>157</v>
       </c>
       <c r="E136" t="s">
-        <v>312</v>
-      </c>
-      <c r="F136" t="s">
-        <v>138</v>
+        <v>158</v>
+      </c>
+      <c r="F136">
+        <v>183</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
@@ -4733,13 +4271,13 @@
         <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>311</v>
+        <v>157</v>
       </c>
       <c r="E137" t="s">
-        <v>313</v>
-      </c>
-      <c r="F137" t="s">
-        <v>139</v>
+        <v>159</v>
+      </c>
+      <c r="F137">
+        <v>157</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -4753,13 +4291,13 @@
         <v>0</v>
       </c>
       <c r="D138" t="s">
-        <v>314</v>
+        <v>160</v>
       </c>
       <c r="E138" t="s">
-        <v>315</v>
-      </c>
-      <c r="F138" t="s">
-        <v>139</v>
+        <v>161</v>
+      </c>
+      <c r="F138">
+        <v>157</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
@@ -4773,13 +4311,13 @@
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>314</v>
+        <v>160</v>
       </c>
       <c r="E139" t="s">
-        <v>316</v>
-      </c>
-      <c r="F139" t="s">
-        <v>140</v>
+        <v>162</v>
+      </c>
+      <c r="F139">
+        <v>122</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -4793,13 +4331,13 @@
         <v>0</v>
       </c>
       <c r="D140" t="s">
-        <v>317</v>
+        <v>163</v>
       </c>
       <c r="E140" t="s">
-        <v>318</v>
-      </c>
-      <c r="F140" t="s">
-        <v>141</v>
+        <v>164</v>
+      </c>
+      <c r="F140">
+        <v>322</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -4813,13 +4351,13 @@
         <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>317</v>
+        <v>163</v>
       </c>
       <c r="E141" t="s">
-        <v>319</v>
-      </c>
-      <c r="F141" t="s">
-        <v>142</v>
+        <v>165</v>
+      </c>
+      <c r="F141">
+        <v>224</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -4833,13 +4371,13 @@
         <v>0</v>
       </c>
       <c r="D142" t="s">
-        <v>320</v>
+        <v>166</v>
       </c>
       <c r="E142" t="s">
-        <v>321</v>
-      </c>
-      <c r="F142" t="s">
-        <v>143</v>
+        <v>167</v>
+      </c>
+      <c r="F142">
+        <v>162</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
@@ -4853,13 +4391,13 @@
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>320</v>
+        <v>166</v>
       </c>
       <c r="E143" t="s">
-        <v>322</v>
-      </c>
-      <c r="F143" t="s">
-        <v>144</v>
+        <v>168</v>
+      </c>
+      <c r="F143">
+        <v>172</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -4873,13 +4411,13 @@
         <v>0</v>
       </c>
       <c r="D144" t="s">
-        <v>323</v>
+        <v>169</v>
       </c>
       <c r="E144" t="s">
-        <v>324</v>
-      </c>
-      <c r="F144" t="s">
-        <v>127</v>
+        <v>170</v>
+      </c>
+      <c r="F144">
+        <v>205</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -4893,13 +4431,13 @@
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>323</v>
+        <v>169</v>
       </c>
       <c r="E145" t="s">
-        <v>325</v>
-      </c>
-      <c r="F145" t="s">
-        <v>145</v>
+        <v>171</v>
+      </c>
+      <c r="F145">
+        <v>193</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -4913,13 +4451,13 @@
         <v>0</v>
       </c>
       <c r="D146" t="s">
-        <v>326</v>
+        <v>172</v>
       </c>
       <c r="E146" t="s">
-        <v>327</v>
-      </c>
-      <c r="F146" t="s">
-        <v>146</v>
+        <v>173</v>
+      </c>
+      <c r="F146">
+        <v>189</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
@@ -4933,13 +4471,13 @@
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>326</v>
+        <v>172</v>
       </c>
       <c r="E147" t="s">
-        <v>328</v>
-      </c>
-      <c r="F147" t="s">
-        <v>147</v>
+        <v>174</v>
+      </c>
+      <c r="F147">
+        <v>208</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
@@ -4953,13 +4491,13 @@
         <v>0</v>
       </c>
       <c r="D148" t="s">
-        <v>329</v>
+        <v>175</v>
       </c>
       <c r="E148" t="s">
-        <v>330</v>
-      </c>
-      <c r="F148" t="s">
-        <v>148</v>
+        <v>176</v>
+      </c>
+      <c r="F148">
+        <v>196</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
@@ -4973,13 +4511,13 @@
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>329</v>
+        <v>175</v>
       </c>
       <c r="E149" t="s">
-        <v>331</v>
-      </c>
-      <c r="F149" t="s">
-        <v>149</v>
+        <v>177</v>
+      </c>
+      <c r="F149">
+        <v>194</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
@@ -4993,13 +4531,13 @@
         <v>0</v>
       </c>
       <c r="D150" t="s">
-        <v>332</v>
+        <v>178</v>
       </c>
       <c r="E150" t="s">
-        <v>333</v>
-      </c>
-      <c r="F150" t="s">
-        <v>150</v>
+        <v>179</v>
+      </c>
+      <c r="F150">
+        <v>326</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
@@ -5013,13 +4551,13 @@
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>332</v>
+        <v>178</v>
       </c>
       <c r="E151" t="s">
-        <v>334</v>
-      </c>
-      <c r="F151" t="s">
-        <v>151</v>
+        <v>180</v>
+      </c>
+      <c r="F151">
+        <v>222</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -5033,13 +4571,13 @@
         <v>0</v>
       </c>
       <c r="D152" t="s">
-        <v>335</v>
+        <v>181</v>
       </c>
       <c r="E152" t="s">
-        <v>336</v>
-      </c>
-      <c r="F152" t="s">
-        <v>108</v>
+        <v>182</v>
+      </c>
+      <c r="F152">
+        <v>180</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
@@ -5053,13 +4591,13 @@
         <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>335</v>
+        <v>181</v>
       </c>
       <c r="E153" t="s">
-        <v>337</v>
-      </c>
-      <c r="F153" t="s">
-        <v>152</v>
+        <v>183</v>
+      </c>
+      <c r="F153">
+        <v>230</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -5073,13 +4611,13 @@
         <v>0</v>
       </c>
       <c r="D154" t="s">
-        <v>338</v>
+        <v>184</v>
       </c>
       <c r="E154" t="s">
-        <v>339</v>
-      </c>
-      <c r="F154" t="s">
-        <v>153</v>
+        <v>185</v>
+      </c>
+      <c r="F154">
+        <v>155</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -5093,13 +4631,13 @@
         <v>1</v>
       </c>
       <c r="D155" t="s">
-        <v>338</v>
+        <v>184</v>
       </c>
       <c r="E155" t="s">
-        <v>340</v>
-      </c>
-      <c r="F155" t="s">
-        <v>146</v>
+        <v>186</v>
+      </c>
+      <c r="F155">
+        <v>189</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -5113,13 +4651,13 @@
         <v>0</v>
       </c>
       <c r="D156" t="s">
-        <v>341</v>
+        <v>187</v>
       </c>
       <c r="E156" t="s">
-        <v>342</v>
-      </c>
-      <c r="F156" t="s">
-        <v>154</v>
+        <v>188</v>
+      </c>
+      <c r="F156">
+        <v>188</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -5133,13 +4671,13 @@
         <v>1</v>
       </c>
       <c r="D157" t="s">
-        <v>341</v>
+        <v>187</v>
       </c>
       <c r="E157" t="s">
-        <v>343</v>
-      </c>
-      <c r="F157" t="s">
-        <v>155</v>
+        <v>189</v>
+      </c>
+      <c r="F157">
+        <v>227</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
@@ -5153,13 +4691,13 @@
         <v>0</v>
       </c>
       <c r="D158" t="s">
-        <v>344</v>
+        <v>190</v>
       </c>
       <c r="E158" t="s">
-        <v>345</v>
-      </c>
-      <c r="F158" t="s">
-        <v>156</v>
+        <v>191</v>
+      </c>
+      <c r="F158">
+        <v>181</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
@@ -5173,13 +4711,13 @@
         <v>1</v>
       </c>
       <c r="D159" t="s">
-        <v>344</v>
+        <v>190</v>
       </c>
       <c r="E159" t="s">
-        <v>346</v>
-      </c>
-      <c r="F159" t="s">
-        <v>157</v>
+        <v>192</v>
+      </c>
+      <c r="F159">
+        <v>200</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -5193,13 +4731,13 @@
         <v>0</v>
       </c>
       <c r="D160" t="s">
-        <v>347</v>
+        <v>193</v>
       </c>
       <c r="E160" t="s">
-        <v>348</v>
-      </c>
-      <c r="F160" t="s">
-        <v>158</v>
+        <v>194</v>
+      </c>
+      <c r="F160">
+        <v>168</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
@@ -5213,13 +4751,13 @@
         <v>1</v>
       </c>
       <c r="D161" t="s">
-        <v>347</v>
+        <v>193</v>
       </c>
       <c r="E161" t="s">
-        <v>349</v>
-      </c>
-      <c r="F161" t="s">
-        <v>159</v>
+        <v>195</v>
+      </c>
+      <c r="F161">
+        <v>259</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
@@ -5233,13 +4771,13 @@
         <v>0</v>
       </c>
       <c r="D162" t="s">
-        <v>350</v>
+        <v>196</v>
       </c>
       <c r="E162" t="s">
-        <v>351</v>
-      </c>
-      <c r="F162" t="s">
-        <v>160</v>
+        <v>197</v>
+      </c>
+      <c r="F162">
+        <v>581</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
@@ -5253,13 +4791,13 @@
         <v>1</v>
       </c>
       <c r="D163" t="s">
-        <v>350</v>
+        <v>196</v>
       </c>
       <c r="E163" t="s">
-        <v>352</v>
-      </c>
-      <c r="F163" t="s">
-        <v>161</v>
+        <v>198</v>
+      </c>
+      <c r="F163">
+        <v>650</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
@@ -5273,13 +4811,13 @@
         <v>0</v>
       </c>
       <c r="D164" t="s">
-        <v>353</v>
+        <v>199</v>
       </c>
       <c r="E164" t="s">
-        <v>354</v>
-      </c>
-      <c r="F164" t="s">
-        <v>162</v>
+        <v>200</v>
+      </c>
+      <c r="F164">
+        <v>635</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
@@ -5293,13 +4831,13 @@
         <v>1</v>
       </c>
       <c r="D165" t="s">
-        <v>353</v>
+        <v>199</v>
       </c>
       <c r="E165" t="s">
-        <v>355</v>
-      </c>
-      <c r="F165" t="s">
-        <v>163</v>
+        <v>201</v>
+      </c>
+      <c r="F165">
+        <v>555</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
@@ -5313,13 +4851,13 @@
         <v>0</v>
       </c>
       <c r="D166" t="s">
-        <v>356</v>
+        <v>202</v>
       </c>
       <c r="E166" t="s">
-        <v>357</v>
-      </c>
-      <c r="F166" t="s">
-        <v>155</v>
+        <v>203</v>
+      </c>
+      <c r="F166">
+        <v>227</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
@@ -5333,13 +4871,13 @@
         <v>1</v>
       </c>
       <c r="D167" t="s">
-        <v>356</v>
+        <v>202</v>
       </c>
       <c r="E167" t="s">
-        <v>358</v>
-      </c>
-      <c r="F167" t="s">
-        <v>164</v>
+        <v>204</v>
+      </c>
+      <c r="F167">
+        <v>307</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
@@ -5353,13 +4891,13 @@
         <v>0</v>
       </c>
       <c r="D168" t="s">
-        <v>359</v>
+        <v>205</v>
       </c>
       <c r="E168" t="s">
-        <v>360</v>
-      </c>
-      <c r="F168" t="s">
-        <v>165</v>
+        <v>206</v>
+      </c>
+      <c r="F168">
+        <v>99</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
@@ -5373,13 +4911,13 @@
         <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>359</v>
+        <v>205</v>
       </c>
       <c r="E169" t="s">
-        <v>361</v>
-      </c>
-      <c r="F169" t="s">
-        <v>166</v>
+        <v>207</v>
+      </c>
+      <c r="F169">
+        <v>86</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
@@ -5393,13 +4931,13 @@
         <v>0</v>
       </c>
       <c r="D170" t="s">
-        <v>362</v>
+        <v>208</v>
       </c>
       <c r="E170" t="s">
-        <v>363</v>
-      </c>
-      <c r="F170" t="s">
-        <v>167</v>
+        <v>209</v>
+      </c>
+      <c r="F170">
+        <v>475</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
@@ -5413,13 +4951,13 @@
         <v>1</v>
       </c>
       <c r="D171" t="s">
-        <v>362</v>
+        <v>208</v>
       </c>
       <c r="E171" t="s">
-        <v>364</v>
-      </c>
-      <c r="F171" t="s">
-        <v>168</v>
+        <v>210</v>
+      </c>
+      <c r="F171">
+        <v>438</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
@@ -5433,13 +4971,13 @@
         <v>0</v>
       </c>
       <c r="D172" t="s">
-        <v>365</v>
+        <v>211</v>
       </c>
       <c r="E172" t="s">
-        <v>366</v>
-      </c>
-      <c r="F172" t="s">
-        <v>169</v>
+        <v>212</v>
+      </c>
+      <c r="F172">
+        <v>255</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
@@ -5453,13 +4991,13 @@
         <v>1</v>
       </c>
       <c r="D173" t="s">
-        <v>365</v>
+        <v>211</v>
       </c>
       <c r="E173" t="s">
-        <v>367</v>
-      </c>
-      <c r="F173" t="s">
-        <v>170</v>
+        <v>213</v>
+      </c>
+      <c r="F173">
+        <v>214</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
@@ -5473,13 +5011,13 @@
         <v>0</v>
       </c>
       <c r="D174" t="s">
-        <v>368</v>
+        <v>214</v>
       </c>
       <c r="E174" t="s">
-        <v>369</v>
-      </c>
-      <c r="F174" t="s">
-        <v>171</v>
+        <v>215</v>
+      </c>
+      <c r="F174">
+        <v>603</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
@@ -5493,13 +5031,13 @@
         <v>1</v>
       </c>
       <c r="D175" t="s">
-        <v>368</v>
+        <v>214</v>
       </c>
       <c r="E175" t="s">
-        <v>370</v>
-      </c>
-      <c r="F175" t="s">
-        <v>172</v>
+        <v>216</v>
+      </c>
+      <c r="F175">
+        <v>751</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
@@ -5513,13 +5051,13 @@
         <v>0</v>
       </c>
       <c r="D176" t="s">
-        <v>371</v>
+        <v>217</v>
       </c>
       <c r="E176" t="s">
-        <v>372</v>
-      </c>
-      <c r="F176" t="s">
-        <v>173</v>
+        <v>218</v>
+      </c>
+      <c r="F176">
+        <v>225</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
@@ -5533,13 +5071,13 @@
         <v>1</v>
       </c>
       <c r="D177" t="s">
-        <v>371</v>
+        <v>217</v>
       </c>
       <c r="E177" t="s">
-        <v>373</v>
-      </c>
-      <c r="F177" t="s">
-        <v>174</v>
+        <v>219</v>
+      </c>
+      <c r="F177">
+        <v>369</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
@@ -5553,13 +5091,13 @@
         <v>0</v>
       </c>
       <c r="D178" t="s">
-        <v>374</v>
+        <v>220</v>
       </c>
       <c r="E178" t="s">
-        <v>375</v>
-      </c>
-      <c r="F178" t="s">
-        <v>175</v>
+        <v>221</v>
+      </c>
+      <c r="F178">
+        <v>526</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -5573,13 +5111,13 @@
         <v>1</v>
       </c>
       <c r="D179" t="s">
-        <v>374</v>
+        <v>220</v>
       </c>
       <c r="E179" t="s">
-        <v>376</v>
-      </c>
-      <c r="F179" t="s">
-        <v>176</v>
+        <v>222</v>
+      </c>
+      <c r="F179">
+        <v>469</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -5593,13 +5131,13 @@
         <v>0</v>
       </c>
       <c r="D180" t="s">
-        <v>377</v>
+        <v>223</v>
       </c>
       <c r="E180" t="s">
-        <v>378</v>
-      </c>
-      <c r="F180" t="s">
-        <v>177</v>
+        <v>224</v>
+      </c>
+      <c r="F180">
+        <v>84</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -5613,13 +5151,13 @@
         <v>1</v>
       </c>
       <c r="D181" t="s">
-        <v>377</v>
+        <v>223</v>
       </c>
       <c r="E181" t="s">
-        <v>379</v>
-      </c>
-      <c r="F181" t="s">
-        <v>165</v>
+        <v>225</v>
+      </c>
+      <c r="F181">
+        <v>99</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
@@ -5633,13 +5171,13 @@
         <v>0</v>
       </c>
       <c r="D182" t="s">
-        <v>380</v>
+        <v>226</v>
       </c>
       <c r="E182" t="s">
-        <v>381</v>
-      </c>
-      <c r="F182" t="s">
-        <v>178</v>
+        <v>227</v>
+      </c>
+      <c r="F182">
+        <v>508</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
@@ -5653,13 +5191,13 @@
         <v>1</v>
       </c>
       <c r="D183" t="s">
-        <v>380</v>
+        <v>226</v>
       </c>
       <c r="E183" t="s">
-        <v>382</v>
-      </c>
-      <c r="F183" t="s">
-        <v>179</v>
+        <v>228</v>
+      </c>
+      <c r="F183">
+        <v>362</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
@@ -5673,13 +5211,13 @@
         <v>0</v>
       </c>
       <c r="D184" t="s">
-        <v>383</v>
+        <v>229</v>
       </c>
       <c r="E184" t="s">
-        <v>384</v>
-      </c>
-      <c r="F184" t="s">
-        <v>180</v>
+        <v>230</v>
+      </c>
+      <c r="F184">
+        <v>151</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -5693,13 +5231,13 @@
         <v>1</v>
       </c>
       <c r="D185" t="s">
-        <v>383</v>
+        <v>229</v>
       </c>
       <c r="E185" t="s">
-        <v>385</v>
-      </c>
-      <c r="F185" t="s">
-        <v>157</v>
+        <v>231</v>
+      </c>
+      <c r="F185">
+        <v>200</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
@@ -5713,13 +5251,13 @@
         <v>0</v>
       </c>
       <c r="D186" t="s">
-        <v>386</v>
+        <v>232</v>
       </c>
       <c r="E186" t="s">
-        <v>387</v>
-      </c>
-      <c r="F186" t="s">
-        <v>181</v>
+        <v>233</v>
+      </c>
+      <c r="F186">
+        <v>522</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
@@ -5733,13 +5271,13 @@
         <v>1</v>
       </c>
       <c r="D187" t="s">
-        <v>386</v>
+        <v>232</v>
       </c>
       <c r="E187" t="s">
-        <v>388</v>
-      </c>
-      <c r="F187" t="s">
-        <v>182</v>
+        <v>234</v>
+      </c>
+      <c r="F187">
+        <v>272</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
@@ -5753,13 +5291,13 @@
         <v>0</v>
       </c>
       <c r="D188" t="s">
-        <v>389</v>
+        <v>235</v>
       </c>
       <c r="E188" t="s">
-        <v>390</v>
-      </c>
-      <c r="F188" t="s">
-        <v>183</v>
+        <v>236</v>
+      </c>
+      <c r="F188">
+        <v>780</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -5773,13 +5311,13 @@
         <v>1</v>
       </c>
       <c r="D189" t="s">
-        <v>389</v>
+        <v>235</v>
       </c>
       <c r="E189" t="s">
-        <v>391</v>
-      </c>
-      <c r="F189" t="s">
-        <v>184</v>
+        <v>237</v>
+      </c>
+      <c r="F189">
+        <v>843</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
@@ -5793,13 +5331,13 @@
         <v>0</v>
       </c>
       <c r="D190" t="s">
-        <v>392</v>
+        <v>238</v>
       </c>
       <c r="E190" t="s">
-        <v>393</v>
-      </c>
-      <c r="F190" t="s">
-        <v>185</v>
+        <v>239</v>
+      </c>
+      <c r="F190">
+        <v>638</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
@@ -5813,13 +5351,13 @@
         <v>1</v>
       </c>
       <c r="D191" t="s">
-        <v>392</v>
+        <v>238</v>
       </c>
       <c r="E191" t="s">
-        <v>394</v>
-      </c>
-      <c r="F191" t="s">
-        <v>186</v>
+        <v>240</v>
+      </c>
+      <c r="F191">
+        <v>705</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
@@ -5833,13 +5371,13 @@
         <v>0</v>
       </c>
       <c r="D192" t="s">
-        <v>395</v>
+        <v>241</v>
       </c>
       <c r="E192" t="s">
-        <v>396</v>
-      </c>
-      <c r="F192" t="s">
-        <v>187</v>
+        <v>242</v>
+      </c>
+      <c r="F192">
+        <v>425</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
@@ -5853,13 +5391,13 @@
         <v>1</v>
       </c>
       <c r="D193" t="s">
-        <v>395</v>
+        <v>241</v>
       </c>
       <c r="E193" t="s">
-        <v>397</v>
-      </c>
-      <c r="F193" t="s">
-        <v>188</v>
+        <v>243</v>
+      </c>
+      <c r="F193">
+        <v>558</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
@@ -5873,13 +5411,13 @@
         <v>0</v>
       </c>
       <c r="D194" t="s">
-        <v>398</v>
+        <v>244</v>
       </c>
       <c r="E194" t="s">
-        <v>399</v>
-      </c>
-      <c r="F194" t="s">
-        <v>189</v>
+        <v>245</v>
+      </c>
+      <c r="F194">
+        <v>250</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
@@ -5893,13 +5431,13 @@
         <v>1</v>
       </c>
       <c r="D195" t="s">
-        <v>398</v>
+        <v>244</v>
       </c>
       <c r="E195" t="s">
-        <v>400</v>
-      </c>
-      <c r="F195" t="s">
-        <v>190</v>
+        <v>246</v>
+      </c>
+      <c r="F195">
+        <v>264</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
@@ -5913,13 +5451,13 @@
         <v>0</v>
       </c>
       <c r="D196" t="s">
-        <v>401</v>
+        <v>247</v>
       </c>
       <c r="E196" t="s">
-        <v>402</v>
-      </c>
-      <c r="F196" t="s">
-        <v>191</v>
+        <v>248</v>
+      </c>
+      <c r="F196">
+        <v>643</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
@@ -5933,13 +5471,13 @@
         <v>1</v>
       </c>
       <c r="D197" t="s">
-        <v>401</v>
+        <v>247</v>
       </c>
       <c r="E197" t="s">
-        <v>403</v>
-      </c>
-      <c r="F197" t="s">
-        <v>192</v>
+        <v>249</v>
+      </c>
+      <c r="F197">
+        <v>790</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
@@ -5953,13 +5491,13 @@
         <v>0</v>
       </c>
       <c r="D198" t="s">
-        <v>404</v>
+        <v>250</v>
       </c>
       <c r="E198" t="s">
-        <v>405</v>
-      </c>
-      <c r="F198" t="s">
-        <v>169</v>
+        <v>251</v>
+      </c>
+      <c r="F198">
+        <v>255</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
@@ -5973,13 +5511,13 @@
         <v>1</v>
       </c>
       <c r="D199" t="s">
-        <v>404</v>
+        <v>250</v>
       </c>
       <c r="E199" t="s">
-        <v>406</v>
-      </c>
-      <c r="F199" t="s">
-        <v>193</v>
+        <v>252</v>
+      </c>
+      <c r="F199">
+        <v>811</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
@@ -5993,13 +5531,13 @@
         <v>0</v>
       </c>
       <c r="D200" t="s">
-        <v>407</v>
+        <v>253</v>
       </c>
       <c r="E200" t="s">
-        <v>408</v>
-      </c>
-      <c r="F200" t="s">
-        <v>194</v>
+        <v>254</v>
+      </c>
+      <c r="F200">
+        <v>546</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
@@ -6013,13 +5551,13 @@
         <v>1</v>
       </c>
       <c r="D201" t="s">
-        <v>407</v>
+        <v>253</v>
       </c>
       <c r="E201" t="s">
-        <v>409</v>
-      </c>
-      <c r="F201" t="s">
-        <v>195</v>
+        <v>255</v>
+      </c>
+      <c r="F201">
+        <v>632</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
@@ -6033,13 +5571,13 @@
         <v>0</v>
       </c>
       <c r="D202" t="s">
-        <v>410</v>
+        <v>256</v>
       </c>
       <c r="E202" t="s">
-        <v>411</v>
-      </c>
-      <c r="F202" t="s">
-        <v>196</v>
+        <v>257</v>
+      </c>
+      <c r="F202">
+        <v>275</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
@@ -6053,13 +5591,13 @@
         <v>1</v>
       </c>
       <c r="D203" t="s">
-        <v>410</v>
+        <v>256</v>
       </c>
       <c r="E203" t="s">
-        <v>412</v>
-      </c>
-      <c r="F203" t="s">
-        <v>170</v>
+        <v>258</v>
+      </c>
+      <c r="F203">
+        <v>214</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
@@ -6073,13 +5611,13 @@
         <v>0</v>
       </c>
       <c r="D204" t="s">
-        <v>413</v>
+        <v>259</v>
       </c>
       <c r="E204" t="s">
-        <v>414</v>
-      </c>
-      <c r="F204" t="s">
-        <v>197</v>
+        <v>260</v>
+      </c>
+      <c r="F204">
+        <v>228</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
@@ -6093,13 +5631,13 @@
         <v>1</v>
       </c>
       <c r="D205" t="s">
-        <v>413</v>
+        <v>259</v>
       </c>
       <c r="E205" t="s">
-        <v>415</v>
-      </c>
-      <c r="F205" t="s">
-        <v>198</v>
+        <v>261</v>
+      </c>
+      <c r="F205">
+        <v>292</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
@@ -6113,13 +5651,13 @@
         <v>0</v>
       </c>
       <c r="D206" t="s">
-        <v>416</v>
+        <v>262</v>
       </c>
       <c r="E206" t="s">
-        <v>417</v>
-      </c>
-      <c r="F206" t="s">
-        <v>120</v>
+        <v>263</v>
+      </c>
+      <c r="F206">
+        <v>298</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
@@ -6133,13 +5671,13 @@
         <v>1</v>
       </c>
       <c r="D207" t="s">
-        <v>416</v>
+        <v>262</v>
       </c>
       <c r="E207" t="s">
-        <v>418</v>
-      </c>
-      <c r="F207" t="s">
-        <v>199</v>
+        <v>264</v>
+      </c>
+      <c r="F207">
+        <v>167</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
@@ -6153,13 +5691,13 @@
         <v>0</v>
       </c>
       <c r="D208" t="s">
-        <v>419</v>
+        <v>265</v>
       </c>
       <c r="E208" t="s">
-        <v>420</v>
-      </c>
-      <c r="F208" t="s">
-        <v>200</v>
+        <v>266</v>
+      </c>
+      <c r="F208">
+        <v>351</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
@@ -6173,13 +5711,13 @@
         <v>1</v>
       </c>
       <c r="D209" t="s">
-        <v>419</v>
+        <v>265</v>
       </c>
       <c r="E209" t="s">
-        <v>421</v>
-      </c>
-      <c r="F209" t="s">
-        <v>164</v>
+        <v>267</v>
+      </c>
+      <c r="F209">
+        <v>307</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
@@ -6193,13 +5731,13 @@
         <v>0</v>
       </c>
       <c r="D210" t="s">
-        <v>422</v>
+        <v>268</v>
       </c>
       <c r="E210" t="s">
-        <v>423</v>
-      </c>
-      <c r="F210" t="s">
-        <v>201</v>
+        <v>269</v>
+      </c>
+      <c r="F210">
+        <v>211</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
@@ -6213,13 +5751,13 @@
         <v>1</v>
       </c>
       <c r="D211" t="s">
-        <v>422</v>
+        <v>268</v>
       </c>
       <c r="E211" t="s">
-        <v>424</v>
-      </c>
-      <c r="F211" t="s">
-        <v>202</v>
+        <v>270</v>
+      </c>
+      <c r="F211">
+        <v>132</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
@@ -6233,13 +5771,13 @@
         <v>0</v>
       </c>
       <c r="D212" t="s">
-        <v>425</v>
+        <v>271</v>
       </c>
       <c r="E212" t="s">
-        <v>426</v>
-      </c>
-      <c r="F212" t="s">
-        <v>120</v>
+        <v>272</v>
+      </c>
+      <c r="F212">
+        <v>298</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
@@ -6253,13 +5791,13 @@
         <v>1</v>
       </c>
       <c r="D213" t="s">
-        <v>425</v>
+        <v>271</v>
       </c>
       <c r="E213" t="s">
-        <v>427</v>
-      </c>
-      <c r="F213" t="s">
-        <v>203</v>
+        <v>273</v>
+      </c>
+      <c r="F213">
+        <v>147</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
@@ -6273,13 +5811,13 @@
         <v>0</v>
       </c>
       <c r="D214" t="s">
-        <v>428</v>
+        <v>274</v>
       </c>
       <c r="E214" t="s">
-        <v>429</v>
-      </c>
-      <c r="F214" t="s">
-        <v>108</v>
+        <v>275</v>
+      </c>
+      <c r="F214">
+        <v>180</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
@@ -6293,13 +5831,13 @@
         <v>1</v>
       </c>
       <c r="D215" t="s">
-        <v>428</v>
+        <v>274</v>
       </c>
       <c r="E215" t="s">
-        <v>430</v>
-      </c>
-      <c r="F215" t="s">
-        <v>204</v>
+        <v>276</v>
+      </c>
+      <c r="F215">
+        <v>152</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
@@ -6313,13 +5851,13 @@
         <v>0</v>
       </c>
       <c r="D216" t="s">
-        <v>431</v>
+        <v>277</v>
       </c>
       <c r="E216" t="s">
-        <v>432</v>
-      </c>
-      <c r="F216" t="s">
-        <v>205</v>
+        <v>278</v>
+      </c>
+      <c r="F216">
+        <v>269</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
@@ -6333,13 +5871,13 @@
         <v>1</v>
       </c>
       <c r="D217" t="s">
-        <v>431</v>
+        <v>277</v>
       </c>
       <c r="E217" t="s">
-        <v>433</v>
-      </c>
-      <c r="F217" t="s">
-        <v>206</v>
+        <v>279</v>
+      </c>
+      <c r="F217">
+        <v>257</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
@@ -6353,13 +5891,13 @@
         <v>0</v>
       </c>
       <c r="D218" t="s">
-        <v>434</v>
+        <v>280</v>
       </c>
       <c r="E218" t="s">
-        <v>435</v>
-      </c>
-      <c r="F218" t="s">
-        <v>108</v>
+        <v>281</v>
+      </c>
+      <c r="F218">
+        <v>180</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
@@ -6373,13 +5911,13 @@
         <v>1</v>
       </c>
       <c r="D219" t="s">
-        <v>434</v>
+        <v>280</v>
       </c>
       <c r="E219" t="s">
-        <v>436</v>
-      </c>
-      <c r="F219" t="s">
-        <v>127</v>
+        <v>282</v>
+      </c>
+      <c r="F219">
+        <v>205</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
@@ -6393,13 +5931,13 @@
         <v>0</v>
       </c>
       <c r="D220" t="s">
-        <v>437</v>
+        <v>283</v>
       </c>
       <c r="E220" t="s">
-        <v>438</v>
-      </c>
-      <c r="F220" t="s">
-        <v>207</v>
+        <v>284</v>
+      </c>
+      <c r="F220">
+        <v>104</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
@@ -6413,13 +5951,13 @@
         <v>1</v>
       </c>
       <c r="D221" t="s">
-        <v>437</v>
+        <v>283</v>
       </c>
       <c r="E221" t="s">
-        <v>439</v>
-      </c>
-      <c r="F221" t="s">
-        <v>123</v>
+        <v>285</v>
+      </c>
+      <c r="F221">
+        <v>48</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
@@ -6433,13 +5971,13 @@
         <v>0</v>
       </c>
       <c r="D222" t="s">
-        <v>440</v>
+        <v>286</v>
       </c>
       <c r="E222" t="s">
-        <v>441</v>
-      </c>
-      <c r="F222" t="s">
-        <v>208</v>
+        <v>287</v>
+      </c>
+      <c r="F222">
+        <v>805</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
@@ -6453,13 +5991,13 @@
         <v>1</v>
       </c>
       <c r="D223" t="s">
-        <v>440</v>
+        <v>286</v>
       </c>
       <c r="E223" t="s">
-        <v>442</v>
-      </c>
-      <c r="F223" t="s">
-        <v>209</v>
+        <v>288</v>
+      </c>
+      <c r="F223">
+        <v>645</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
@@ -6473,13 +6011,13 @@
         <v>0</v>
       </c>
       <c r="D224" t="s">
-        <v>443</v>
+        <v>289</v>
       </c>
       <c r="E224" t="s">
-        <v>444</v>
-      </c>
-      <c r="F224" t="s">
-        <v>210</v>
+        <v>290</v>
+      </c>
+      <c r="F224">
+        <v>334</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
@@ -6493,13 +6031,13 @@
         <v>1</v>
       </c>
       <c r="D225" t="s">
-        <v>443</v>
+        <v>289</v>
       </c>
       <c r="E225" t="s">
-        <v>445</v>
-      </c>
-      <c r="F225" t="s">
-        <v>211</v>
+        <v>291</v>
+      </c>
+      <c r="F225">
+        <v>246</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
@@ -6513,13 +6051,13 @@
         <v>0</v>
       </c>
       <c r="D226" t="s">
-        <v>446</v>
+        <v>292</v>
       </c>
       <c r="E226" t="s">
-        <v>447</v>
-      </c>
-      <c r="F226" t="s">
-        <v>212</v>
+        <v>293</v>
+      </c>
+      <c r="F226">
+        <v>530</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
@@ -6533,13 +6071,13 @@
         <v>1</v>
       </c>
       <c r="D227" t="s">
-        <v>446</v>
+        <v>292</v>
       </c>
       <c r="E227" t="s">
-        <v>448</v>
-      </c>
-      <c r="F227" t="s">
-        <v>213</v>
+        <v>294</v>
+      </c>
+      <c r="F227">
+        <v>505</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
@@ -6553,13 +6091,13 @@
         <v>0</v>
       </c>
       <c r="D228" t="s">
-        <v>449</v>
+        <v>295</v>
       </c>
       <c r="E228" t="s">
+        <v>296</v>
+      </c>
+      <c r="F228">
         <v>450</v>
-      </c>
-      <c r="F228" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
@@ -6573,13 +6111,13 @@
         <v>1</v>
       </c>
       <c r="D229" t="s">
-        <v>449</v>
+        <v>295</v>
       </c>
       <c r="E229" t="s">
-        <v>451</v>
-      </c>
-      <c r="F229" t="s">
-        <v>215</v>
+        <v>297</v>
+      </c>
+      <c r="F229">
+        <v>525</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
@@ -6593,13 +6131,13 @@
         <v>0</v>
       </c>
       <c r="D230" t="s">
-        <v>452</v>
+        <v>298</v>
       </c>
       <c r="E230" t="s">
-        <v>453</v>
-      </c>
-      <c r="F230" t="s">
-        <v>216</v>
+        <v>299</v>
+      </c>
+      <c r="F230">
+        <v>433</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
@@ -6613,13 +6151,13 @@
         <v>1</v>
       </c>
       <c r="D231" t="s">
-        <v>452</v>
+        <v>298</v>
       </c>
       <c r="E231" t="s">
-        <v>454</v>
-      </c>
-      <c r="F231" t="s">
-        <v>217</v>
+        <v>300</v>
+      </c>
+      <c r="F231">
+        <v>403</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
@@ -6633,13 +6171,13 @@
         <v>0</v>
       </c>
       <c r="D232" t="s">
-        <v>455</v>
+        <v>301</v>
       </c>
       <c r="E232" t="s">
-        <v>456</v>
-      </c>
-      <c r="F232" t="s">
-        <v>218</v>
+        <v>302</v>
+      </c>
+      <c r="F232">
+        <v>590</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
@@ -6653,13 +6191,13 @@
         <v>1</v>
       </c>
       <c r="D233" t="s">
-        <v>455</v>
+        <v>301</v>
       </c>
       <c r="E233" t="s">
-        <v>457</v>
-      </c>
-      <c r="F233" t="s">
-        <v>219</v>
+        <v>303</v>
+      </c>
+      <c r="F233">
+        <v>538</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
@@ -6673,13 +6211,13 @@
         <v>0</v>
       </c>
       <c r="D234" t="s">
-        <v>458</v>
+        <v>304</v>
       </c>
       <c r="E234" t="s">
-        <v>459</v>
-      </c>
-      <c r="F234" t="s">
-        <v>197</v>
+        <v>305</v>
+      </c>
+      <c r="F234">
+        <v>228</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
@@ -6693,13 +6231,13 @@
         <v>1</v>
       </c>
       <c r="D235" t="s">
-        <v>458</v>
+        <v>304</v>
       </c>
       <c r="E235" t="s">
-        <v>460</v>
-      </c>
-      <c r="F235" t="s">
-        <v>220</v>
+        <v>306</v>
+      </c>
+      <c r="F235">
+        <v>532</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
@@ -6713,13 +6251,13 @@
         <v>0</v>
       </c>
       <c r="D236" t="s">
-        <v>461</v>
+        <v>307</v>
       </c>
       <c r="E236" t="s">
-        <v>462</v>
-      </c>
-      <c r="F236" t="s">
-        <v>221</v>
+        <v>308</v>
+      </c>
+      <c r="F236">
+        <v>368</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
@@ -6733,13 +6271,13 @@
         <v>1</v>
       </c>
       <c r="D237" t="s">
-        <v>461</v>
+        <v>307</v>
       </c>
       <c r="E237" t="s">
-        <v>463</v>
-      </c>
-      <c r="F237" t="s">
-        <v>222</v>
+        <v>309</v>
+      </c>
+      <c r="F237">
+        <v>722</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
@@ -6753,13 +6291,13 @@
         <v>0</v>
       </c>
       <c r="D238" t="s">
-        <v>464</v>
+        <v>310</v>
       </c>
       <c r="E238" t="s">
-        <v>465</v>
-      </c>
-      <c r="F238" t="s">
-        <v>223</v>
+        <v>311</v>
+      </c>
+      <c r="F238">
+        <v>481</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
@@ -6773,13 +6311,13 @@
         <v>1</v>
       </c>
       <c r="D239" t="s">
-        <v>464</v>
+        <v>310</v>
       </c>
       <c r="E239" t="s">
-        <v>466</v>
-      </c>
-      <c r="F239" t="s">
-        <v>224</v>
+        <v>312</v>
+      </c>
+      <c r="F239">
+        <v>566</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
@@ -6793,13 +6331,13 @@
         <v>0</v>
       </c>
       <c r="D240" t="s">
-        <v>467</v>
+        <v>313</v>
       </c>
       <c r="E240" t="s">
-        <v>468</v>
-      </c>
-      <c r="F240" t="s">
-        <v>225</v>
+        <v>314</v>
+      </c>
+      <c r="F240">
+        <v>759</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
@@ -6813,13 +6351,13 @@
         <v>1</v>
       </c>
       <c r="D241" t="s">
-        <v>467</v>
+        <v>313</v>
       </c>
       <c r="E241" t="s">
-        <v>469</v>
-      </c>
-      <c r="F241" t="s">
-        <v>226</v>
+        <v>315</v>
+      </c>
+      <c r="F241">
+        <v>337</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
@@ -6833,13 +6371,13 @@
         <v>0</v>
       </c>
       <c r="D242" t="s">
-        <v>470</v>
+        <v>316</v>
       </c>
       <c r="E242" t="s">
-        <v>471</v>
-      </c>
-      <c r="F242" t="s">
-        <v>227</v>
+        <v>317</v>
+      </c>
+      <c r="F242">
+        <v>402</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
@@ -6853,13 +6391,13 @@
         <v>1</v>
       </c>
       <c r="D243" t="s">
-        <v>470</v>
+        <v>316</v>
       </c>
       <c r="E243" t="s">
-        <v>472</v>
-      </c>
-      <c r="F243" t="s">
-        <v>228</v>
+        <v>318</v>
+      </c>
+      <c r="F243">
+        <v>536</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
@@ -6873,13 +6411,13 @@
         <v>0</v>
       </c>
       <c r="D244" t="s">
-        <v>473</v>
+        <v>319</v>
       </c>
       <c r="E244" t="s">
-        <v>474</v>
-      </c>
-      <c r="F244" t="s">
-        <v>164</v>
+        <v>320</v>
+      </c>
+      <c r="F244">
+        <v>307</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
@@ -6893,13 +6431,13 @@
         <v>1</v>
       </c>
       <c r="D245" t="s">
-        <v>473</v>
+        <v>319</v>
       </c>
       <c r="E245" t="s">
-        <v>475</v>
-      </c>
-      <c r="F245" t="s">
-        <v>229</v>
+        <v>321</v>
+      </c>
+      <c r="F245">
+        <v>485</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
@@ -6913,13 +6451,13 @@
         <v>0</v>
       </c>
       <c r="D246" t="s">
-        <v>476</v>
+        <v>322</v>
       </c>
       <c r="E246" t="s">
-        <v>477</v>
-      </c>
-      <c r="F246" t="s">
-        <v>230</v>
+        <v>323</v>
+      </c>
+      <c r="F246">
+        <v>494</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
@@ -6933,13 +6471,13 @@
         <v>1</v>
       </c>
       <c r="D247" t="s">
-        <v>476</v>
+        <v>322</v>
       </c>
       <c r="E247" t="s">
-        <v>478</v>
-      </c>
-      <c r="F247" t="s">
-        <v>231</v>
+        <v>324</v>
+      </c>
+      <c r="F247">
+        <v>451</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
@@ -6953,13 +6491,13 @@
         <v>0</v>
       </c>
       <c r="D248" t="s">
-        <v>479</v>
+        <v>325</v>
       </c>
       <c r="E248" t="s">
-        <v>480</v>
-      </c>
-      <c r="F248" t="s">
-        <v>232</v>
+        <v>326</v>
+      </c>
+      <c r="F248">
+        <v>289</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
@@ -6973,13 +6511,13 @@
         <v>1</v>
       </c>
       <c r="D249" t="s">
-        <v>479</v>
+        <v>325</v>
       </c>
       <c r="E249" t="s">
-        <v>481</v>
-      </c>
-      <c r="F249" t="s">
-        <v>233</v>
+        <v>327</v>
+      </c>
+      <c r="F249">
+        <v>456</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
@@ -6993,13 +6531,13 @@
         <v>0</v>
       </c>
       <c r="D250" t="s">
-        <v>482</v>
+        <v>328</v>
       </c>
       <c r="E250" t="s">
-        <v>483</v>
-      </c>
-      <c r="F250" t="s">
-        <v>145</v>
+        <v>329</v>
+      </c>
+      <c r="F250">
+        <v>193</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
@@ -7013,13 +6551,13 @@
         <v>1</v>
       </c>
       <c r="D251" t="s">
-        <v>482</v>
+        <v>328</v>
       </c>
       <c r="E251" t="s">
-        <v>484</v>
-      </c>
-      <c r="F251" t="s">
-        <v>234</v>
+        <v>330</v>
+      </c>
+      <c r="F251">
+        <v>177</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
@@ -7033,13 +6571,13 @@
         <v>0</v>
       </c>
       <c r="D252" t="s">
-        <v>485</v>
+        <v>331</v>
       </c>
       <c r="E252" t="s">
-        <v>486</v>
-      </c>
-      <c r="F252" t="s">
-        <v>235</v>
+        <v>332</v>
+      </c>
+      <c r="F252">
+        <v>133</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
@@ -7053,13 +6591,13 @@
         <v>1</v>
       </c>
       <c r="D253" t="s">
-        <v>485</v>
+        <v>331</v>
       </c>
       <c r="E253" t="s">
-        <v>487</v>
-      </c>
-      <c r="F253" t="s">
-        <v>236</v>
+        <v>333</v>
+      </c>
+      <c r="F253">
+        <v>213</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
@@ -7073,13 +6611,13 @@
         <v>0</v>
       </c>
       <c r="D254" t="s">
-        <v>488</v>
+        <v>334</v>
       </c>
       <c r="E254" t="s">
-        <v>489</v>
-      </c>
-      <c r="F254" t="s">
-        <v>237</v>
+        <v>335</v>
+      </c>
+      <c r="F254">
+        <v>423</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
@@ -7093,13 +6631,13 @@
         <v>1</v>
       </c>
       <c r="D255" t="s">
-        <v>488</v>
+        <v>334</v>
       </c>
       <c r="E255" t="s">
-        <v>490</v>
-      </c>
-      <c r="F255" t="s">
-        <v>238</v>
+        <v>336</v>
+      </c>
+      <c r="F255">
+        <v>626</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
@@ -7113,13 +6651,13 @@
         <v>0</v>
       </c>
       <c r="D256" t="s">
-        <v>491</v>
+        <v>337</v>
       </c>
       <c r="E256" t="s">
-        <v>492</v>
-      </c>
-      <c r="F256" t="s">
-        <v>239</v>
+        <v>338</v>
+      </c>
+      <c r="F256">
+        <v>627</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
@@ -7133,13 +6671,13 @@
         <v>1</v>
       </c>
       <c r="D257" t="s">
-        <v>491</v>
+        <v>337</v>
       </c>
       <c r="E257" t="s">
-        <v>493</v>
-      </c>
-      <c r="F257" t="s">
-        <v>240</v>
+        <v>339</v>
+      </c>
+      <c r="F257">
+        <v>757</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
@@ -7153,13 +6691,13 @@
         <v>0</v>
       </c>
       <c r="D258" t="s">
-        <v>494</v>
+        <v>340</v>
       </c>
       <c r="E258" t="s">
-        <v>495</v>
-      </c>
-      <c r="F258" t="s">
-        <v>241</v>
+        <v>341</v>
+      </c>
+      <c r="F258">
+        <v>287</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.2">
@@ -7173,13 +6711,13 @@
         <v>1</v>
       </c>
       <c r="D259" t="s">
-        <v>494</v>
+        <v>340</v>
       </c>
       <c r="E259" t="s">
-        <v>496</v>
-      </c>
-      <c r="F259" t="s">
-        <v>216</v>
+        <v>342</v>
+      </c>
+      <c r="F259">
+        <v>433</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
@@ -7193,13 +6731,13 @@
         <v>0</v>
       </c>
       <c r="D260" t="s">
-        <v>497</v>
+        <v>343</v>
       </c>
       <c r="E260" t="s">
-        <v>498</v>
-      </c>
-      <c r="F260" t="s">
-        <v>242</v>
+        <v>344</v>
+      </c>
+      <c r="F260">
+        <v>615</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
@@ -7213,13 +6751,13 @@
         <v>1</v>
       </c>
       <c r="D261" t="s">
-        <v>497</v>
+        <v>343</v>
       </c>
       <c r="E261" t="s">
-        <v>499</v>
-      </c>
-      <c r="F261" t="s">
-        <v>243</v>
+        <v>345</v>
+      </c>
+      <c r="F261">
+        <v>458</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.2">
@@ -7233,13 +6771,13 @@
         <v>0</v>
       </c>
       <c r="D262" t="s">
-        <v>500</v>
+        <v>346</v>
       </c>
       <c r="E262" t="s">
-        <v>501</v>
-      </c>
-      <c r="F262" t="s">
-        <v>137</v>
+        <v>347</v>
+      </c>
+      <c r="F262">
+        <v>215</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.2">
@@ -7253,13 +6791,13 @@
         <v>1</v>
       </c>
       <c r="D263" t="s">
-        <v>500</v>
+        <v>346</v>
       </c>
       <c r="E263" t="s">
-        <v>502</v>
-      </c>
-      <c r="F263" t="s">
-        <v>244</v>
+        <v>348</v>
+      </c>
+      <c r="F263">
+        <v>301</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.2">
@@ -7273,13 +6811,13 @@
         <v>0</v>
       </c>
       <c r="D264" t="s">
-        <v>503</v>
+        <v>349</v>
       </c>
       <c r="E264" t="s">
-        <v>504</v>
-      </c>
-      <c r="F264" t="s">
-        <v>245</v>
+        <v>350</v>
+      </c>
+      <c r="F264">
+        <v>297</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.2">
@@ -7293,13 +6831,13 @@
         <v>1</v>
       </c>
       <c r="D265" t="s">
-        <v>503</v>
+        <v>349</v>
       </c>
       <c r="E265" t="s">
-        <v>505</v>
-      </c>
-      <c r="F265" t="s">
-        <v>190</v>
+        <v>351</v>
+      </c>
+      <c r="F265">
+        <v>264</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
@@ -7313,13 +6851,13 @@
         <v>0</v>
       </c>
       <c r="D266" t="s">
-        <v>506</v>
+        <v>352</v>
       </c>
       <c r="E266" t="s">
-        <v>507</v>
-      </c>
-      <c r="F266" t="s">
-        <v>246</v>
+        <v>353</v>
+      </c>
+      <c r="F266">
+        <v>245</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.2">
@@ -7333,13 +6871,13 @@
         <v>1</v>
       </c>
       <c r="D267" t="s">
-        <v>506</v>
+        <v>352</v>
       </c>
       <c r="E267" t="s">
-        <v>508</v>
-      </c>
-      <c r="F267" t="s">
-        <v>247</v>
+        <v>354</v>
+      </c>
+      <c r="F267">
+        <v>204</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
@@ -7353,13 +6891,13 @@
         <v>0</v>
       </c>
       <c r="D268" t="s">
-        <v>509</v>
+        <v>355</v>
       </c>
       <c r="E268" t="s">
-        <v>510</v>
-      </c>
-      <c r="F268" t="s">
-        <v>248</v>
+        <v>356</v>
+      </c>
+      <c r="F268">
+        <v>414</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
@@ -7373,13 +6911,13 @@
         <v>1</v>
       </c>
       <c r="D269" t="s">
-        <v>509</v>
+        <v>355</v>
       </c>
       <c r="E269" t="s">
-        <v>511</v>
-      </c>
-      <c r="F269" t="s">
-        <v>249</v>
+        <v>357</v>
+      </c>
+      <c r="F269">
+        <v>390</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
@@ -7393,13 +6931,13 @@
         <v>0</v>
       </c>
       <c r="D270" t="s">
-        <v>512</v>
+        <v>358</v>
       </c>
       <c r="E270" t="s">
-        <v>513</v>
-      </c>
-      <c r="F270" t="s">
-        <v>250</v>
+        <v>359</v>
+      </c>
+      <c r="F270">
+        <v>430</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
@@ -7413,13 +6951,13 @@
         <v>1</v>
       </c>
       <c r="D271" t="s">
-        <v>512</v>
+        <v>358</v>
       </c>
       <c r="E271" t="s">
-        <v>514</v>
-      </c>
-      <c r="F271" t="s">
-        <v>251</v>
+        <v>360</v>
+      </c>
+      <c r="F271">
+        <v>527</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
@@ -7433,13 +6971,13 @@
         <v>0</v>
       </c>
       <c r="D272" t="s">
-        <v>515</v>
+        <v>361</v>
       </c>
       <c r="E272" t="s">
-        <v>516</v>
-      </c>
-      <c r="F272" t="s">
-        <v>252</v>
+        <v>362</v>
+      </c>
+      <c r="F272">
+        <v>372</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.2">
@@ -7453,13 +6991,13 @@
         <v>1</v>
       </c>
       <c r="D273" t="s">
-        <v>515</v>
+        <v>361</v>
       </c>
       <c r="E273" t="s">
-        <v>517</v>
-      </c>
-      <c r="F273" t="s">
-        <v>253</v>
+        <v>363</v>
+      </c>
+      <c r="F273">
+        <v>459</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.2">
@@ -7473,13 +7011,13 @@
         <v>0</v>
       </c>
       <c r="D274" t="s">
-        <v>518</v>
+        <v>364</v>
       </c>
       <c r="E274" t="s">
-        <v>519</v>
-      </c>
-      <c r="F274" t="s">
-        <v>254</v>
+        <v>365</v>
+      </c>
+      <c r="F274">
+        <v>373</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.2">
@@ -7493,13 +7031,13 @@
         <v>1</v>
       </c>
       <c r="D275" t="s">
-        <v>518</v>
+        <v>364</v>
       </c>
       <c r="E275" t="s">
-        <v>520</v>
-      </c>
-      <c r="F275" t="s">
-        <v>255</v>
+        <v>366</v>
+      </c>
+      <c r="F275">
+        <v>486</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.2">
@@ -7513,13 +7051,13 @@
         <v>0</v>
       </c>
       <c r="D276" t="s">
-        <v>521</v>
+        <v>367</v>
       </c>
       <c r="E276" t="s">
-        <v>522</v>
-      </c>
-      <c r="F276" t="s">
-        <v>256</v>
+        <v>368</v>
+      </c>
+      <c r="F276">
+        <v>173</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.2">
@@ -7533,13 +7071,13 @@
         <v>1</v>
       </c>
       <c r="D277" t="s">
-        <v>521</v>
+        <v>367</v>
       </c>
       <c r="E277" t="s">
-        <v>523</v>
-      </c>
-      <c r="F277" t="s">
-        <v>109</v>
+        <v>369</v>
+      </c>
+      <c r="F277">
+        <v>190</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.2">
@@ -7553,13 +7091,13 @@
         <v>0</v>
       </c>
       <c r="D278" t="s">
-        <v>524</v>
+        <v>370</v>
       </c>
       <c r="E278" t="s">
-        <v>525</v>
-      </c>
-      <c r="F278" t="s">
-        <v>257</v>
+        <v>371</v>
+      </c>
+      <c r="F278">
+        <v>359</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.2">
@@ -7573,13 +7111,13 @@
         <v>1</v>
       </c>
       <c r="D279" t="s">
-        <v>524</v>
+        <v>370</v>
       </c>
       <c r="E279" t="s">
-        <v>526</v>
-      </c>
-      <c r="F279" t="s">
-        <v>258</v>
+        <v>372</v>
+      </c>
+      <c r="F279">
+        <v>321</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.2">
@@ -7593,13 +7131,13 @@
         <v>0</v>
       </c>
       <c r="D280" t="s">
-        <v>527</v>
+        <v>373</v>
       </c>
       <c r="E280" t="s">
-        <v>528</v>
-      </c>
-      <c r="F280" t="s">
-        <v>259</v>
+        <v>374</v>
+      </c>
+      <c r="F280">
+        <v>335</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.2">
@@ -7613,13 +7151,13 @@
         <v>1</v>
       </c>
       <c r="D281" t="s">
-        <v>527</v>
+        <v>373</v>
       </c>
       <c r="E281" t="s">
-        <v>529</v>
-      </c>
-      <c r="F281" t="s">
-        <v>121</v>
+        <v>375</v>
+      </c>
+      <c r="F281">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Text second version finished
Added renders for setup and text was read a second time with help from D.H.
</commit_message>
<xml_diff>
--- a/code/Vision/Datasets/labels/labels5.xlsx
+++ b/code/Vision/Datasets/labels/labels5.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsdepauw/Documents/Lars.nosync/Documents/School/1Ma ing/Masterproef/TWI/code/Vision/Datasets/labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AF20F0-B69E-4A43-9A45-B9DE222F5155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F8C11-4296-C840-9A21-993A756E3B0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="-20400" windowWidth="26840" windowHeight="15940" xr2:uid="{7C2D2E37-B908-3941-8EC8-7D93A5E6F16B}"/>
+    <workbookView xWindow="2920" yWindow="1980" windowWidth="26840" windowHeight="15940" xr2:uid="{7C2D2E37-B908-3941-8EC8-7D93A5E6F16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="382">
   <si>
     <t>bullet</t>
   </si>
@@ -1161,6 +1162,24 @@
   </si>
   <si>
     <t>b_019_p_010_l_000_b.png</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>class 0</t>
+  </si>
+  <si>
+    <t>class 1</t>
+  </si>
+  <si>
+    <t>class 2</t>
+  </si>
+  <si>
+    <t>all labels</t>
+  </si>
+  <si>
+    <t>first 5 batches</t>
   </si>
 </sst>
 </file>
@@ -1225,6 +1244,1742 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Class distribution for all inserts</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>146</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EEBF-E34A-ABD5-F6D31854204B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Class distribution</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> for first 5 batches</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$7:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-900A-424A-9C0E-F49C693CD329}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2691D71C-E2B1-E847-9124-F318C45F9D5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31C237D9-6961-6E4A-A453-9C3EA2B9C31A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1527,7 +3282,7 @@
   <dimension ref="A1:F281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7163,4 +8918,2599 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2A913D-C45F-AC41-8287-B680F03D4E7D}">
+  <dimension ref="A1:D281"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>50.73</v>
+      </c>
+      <c r="B2">
+        <f>IF(A2&lt;130,0,IF(A2&lt;230,1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF($B$2:$B$281,0)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>57.122</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">IF(A3&lt;130,0,IF(A3&lt;230,1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D3">
+        <f>COUNTIF($B$2:$B$281,1)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>46.984999999999999</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D4">
+        <f>COUNTIF($B$2:$B$281,2)</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>68.903999999999996</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>35.348999999999997</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>32.594000000000001</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>377</v>
+      </c>
+      <c r="D7">
+        <f>COUNTIF($B$2:$B$101,0)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>38.79</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>378</v>
+      </c>
+      <c r="D8">
+        <f>COUNTIF($B$2:$B$101,1)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>47.353999999999999</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>379</v>
+      </c>
+      <c r="D9">
+        <f>COUNTIF($B$2:$B$101,2)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>42.637</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>44.158999999999999</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>40.957999999999998</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>40.505000000000003</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>34.71</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>44.46</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>75.510000000000005</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>37.774999999999999</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>39.883000000000003</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>53.984000000000002</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>43.45</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>51.164000000000001</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>44.768999999999998</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>55.622</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>55.427999999999997</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>46.991</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>40.301000000000002</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>27.945</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>31.759</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>44.09</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>41.805</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>54.143999999999998</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>42.021999999999998</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>70.105000000000004</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>76.501999999999995</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>58.457000000000001</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>72.137</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>108.938</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>136.44200000000001</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>114.246</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>69.489999999999995</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>157.529</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>150.964</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>163.71</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>250.45099999999999</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>176.70699999999999</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>272.12599999999998</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>159.685</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>262.48700000000002</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>202.03200000000001</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>161.91300000000001</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>389.15</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>287.17</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>172.22200000000001</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>143.72300000000001</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>162.71199999999999</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>147.59100000000001</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>177.483</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>141.84</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>168.27199999999999</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>164.79</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>170.90299999999999</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>194.83199999999999</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>236.77699999999999</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>279.31799999999998</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>234.07400000000001</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>212.64400000000001</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B130" si="1">IF(A67&lt;130,0,IF(A67&lt;230,1,2))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>321.149</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>226.673</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>268.22699999999998</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>250.97900000000001</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>157.04</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>227.3</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>180.68799999999999</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
+        <v>192.24799999999999</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
+        <v>252.178</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="2">
+        <v>245.24299999999999</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>211.89599999999999</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>219.11600000000001</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>126.831</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>242.11199999999999</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
+        <v>342.27199999999999</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="2">
+        <v>240.197</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>451.91500000000002</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="2">
+        <v>309.03800000000001</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="2">
+        <v>348.46899999999999</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="2">
+        <v>409.86500000000001</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="2">
+        <v>368.471</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
+        <v>332.01600000000002</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
+        <v>249.69499999999999</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
+        <v>311.233</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
+        <v>243.72499999999999</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="2">
+        <v>335.22300000000001</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
+        <v>394.68400000000003</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
+        <v>270.416</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
+        <v>466.95600000000002</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
+        <v>399.02499999999998</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>484.96300000000002</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>536.96600000000001</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
+        <v>311.99700000000001</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="2">
+        <v>451.31700000000001</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>358</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>254</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>180</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>190</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>452</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>499</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>572</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>236</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>150</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>244</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>570</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>815</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>577</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>477</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>298</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>219</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>190</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>169</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>48</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>309</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>283</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>260</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>190</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>205</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>98</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>57</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>238</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>137</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>285</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>281</v>
+      </c>
+      <c r="B131">
+        <f t="shared" ref="B131:B194" si="2">IF(A131&lt;130,0,IF(A131&lt;230,1,2))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>251</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>154</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>136</v>
+      </c>
+      <c r="B134">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>215</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>183</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>157</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>157</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>122</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>322</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>224</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>162</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>172</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>205</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>193</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>189</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>208</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>196</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>194</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>326</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>222</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>180</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>230</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>155</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>189</v>
+      </c>
+      <c r="B155">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>188</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>227</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>181</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>200</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>168</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>259</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>581</v>
+      </c>
+      <c r="B162">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>650</v>
+      </c>
+      <c r="B163">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>635</v>
+      </c>
+      <c r="B164">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>555</v>
+      </c>
+      <c r="B165">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>227</v>
+      </c>
+      <c r="B166">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>307</v>
+      </c>
+      <c r="B167">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>99</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>86</v>
+      </c>
+      <c r="B169">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>475</v>
+      </c>
+      <c r="B170">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>438</v>
+      </c>
+      <c r="B171">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>255</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>214</v>
+      </c>
+      <c r="B173">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>603</v>
+      </c>
+      <c r="B174">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>751</v>
+      </c>
+      <c r="B175">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>225</v>
+      </c>
+      <c r="B176">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>369</v>
+      </c>
+      <c r="B177">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>526</v>
+      </c>
+      <c r="B178">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>469</v>
+      </c>
+      <c r="B179">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>84</v>
+      </c>
+      <c r="B180">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>99</v>
+      </c>
+      <c r="B181">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>508</v>
+      </c>
+      <c r="B182">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>362</v>
+      </c>
+      <c r="B183">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>151</v>
+      </c>
+      <c r="B184">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>200</v>
+      </c>
+      <c r="B185">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>522</v>
+      </c>
+      <c r="B186">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>272</v>
+      </c>
+      <c r="B187">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>780</v>
+      </c>
+      <c r="B188">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>843</v>
+      </c>
+      <c r="B189">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>638</v>
+      </c>
+      <c r="B190">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>705</v>
+      </c>
+      <c r="B191">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>425</v>
+      </c>
+      <c r="B192">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>558</v>
+      </c>
+      <c r="B193">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>250</v>
+      </c>
+      <c r="B194">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>264</v>
+      </c>
+      <c r="B195">
+        <f t="shared" ref="B195:B258" si="3">IF(A195&lt;130,0,IF(A195&lt;230,1,2))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>643</v>
+      </c>
+      <c r="B196">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>790</v>
+      </c>
+      <c r="B197">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>255</v>
+      </c>
+      <c r="B198">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>811</v>
+      </c>
+      <c r="B199">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>546</v>
+      </c>
+      <c r="B200">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>632</v>
+      </c>
+      <c r="B201">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>275</v>
+      </c>
+      <c r="B202">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>214</v>
+      </c>
+      <c r="B203">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>228</v>
+      </c>
+      <c r="B204">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>292</v>
+      </c>
+      <c r="B205">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>298</v>
+      </c>
+      <c r="B206">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>167</v>
+      </c>
+      <c r="B207">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>351</v>
+      </c>
+      <c r="B208">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>307</v>
+      </c>
+      <c r="B209">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>211</v>
+      </c>
+      <c r="B210">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>132</v>
+      </c>
+      <c r="B211">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>298</v>
+      </c>
+      <c r="B212">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>147</v>
+      </c>
+      <c r="B213">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>180</v>
+      </c>
+      <c r="B214">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>152</v>
+      </c>
+      <c r="B215">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>269</v>
+      </c>
+      <c r="B216">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>257</v>
+      </c>
+      <c r="B217">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>180</v>
+      </c>
+      <c r="B218">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>205</v>
+      </c>
+      <c r="B219">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>104</v>
+      </c>
+      <c r="B220">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>48</v>
+      </c>
+      <c r="B221">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>805</v>
+      </c>
+      <c r="B222">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>645</v>
+      </c>
+      <c r="B223">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>334</v>
+      </c>
+      <c r="B224">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>246</v>
+      </c>
+      <c r="B225">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>530</v>
+      </c>
+      <c r="B226">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>505</v>
+      </c>
+      <c r="B227">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>450</v>
+      </c>
+      <c r="B228">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>525</v>
+      </c>
+      <c r="B229">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>433</v>
+      </c>
+      <c r="B230">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>403</v>
+      </c>
+      <c r="B231">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>590</v>
+      </c>
+      <c r="B232">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>538</v>
+      </c>
+      <c r="B233">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>228</v>
+      </c>
+      <c r="B234">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>532</v>
+      </c>
+      <c r="B235">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>368</v>
+      </c>
+      <c r="B236">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>722</v>
+      </c>
+      <c r="B237">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>481</v>
+      </c>
+      <c r="B238">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>566</v>
+      </c>
+      <c r="B239">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>759</v>
+      </c>
+      <c r="B240">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>337</v>
+      </c>
+      <c r="B241">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>402</v>
+      </c>
+      <c r="B242">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>536</v>
+      </c>
+      <c r="B243">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>307</v>
+      </c>
+      <c r="B244">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>485</v>
+      </c>
+      <c r="B245">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>494</v>
+      </c>
+      <c r="B246">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>451</v>
+      </c>
+      <c r="B247">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>289</v>
+      </c>
+      <c r="B248">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>456</v>
+      </c>
+      <c r="B249">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>193</v>
+      </c>
+      <c r="B250">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>177</v>
+      </c>
+      <c r="B251">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>133</v>
+      </c>
+      <c r="B252">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>213</v>
+      </c>
+      <c r="B253">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>423</v>
+      </c>
+      <c r="B254">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>626</v>
+      </c>
+      <c r="B255">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>627</v>
+      </c>
+      <c r="B256">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>757</v>
+      </c>
+      <c r="B257">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>287</v>
+      </c>
+      <c r="B258">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>433</v>
+      </c>
+      <c r="B259">
+        <f t="shared" ref="B259:B281" si="4">IF(A259&lt;130,0,IF(A259&lt;230,1,2))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>615</v>
+      </c>
+      <c r="B260">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>458</v>
+      </c>
+      <c r="B261">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>215</v>
+      </c>
+      <c r="B262">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>301</v>
+      </c>
+      <c r="B263">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>297</v>
+      </c>
+      <c r="B264">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>264</v>
+      </c>
+      <c r="B265">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>245</v>
+      </c>
+      <c r="B266">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>204</v>
+      </c>
+      <c r="B267">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>414</v>
+      </c>
+      <c r="B268">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>390</v>
+      </c>
+      <c r="B269">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>430</v>
+      </c>
+      <c r="B270">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>527</v>
+      </c>
+      <c r="B271">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>372</v>
+      </c>
+      <c r="B272">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>459</v>
+      </c>
+      <c r="B273">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>373</v>
+      </c>
+      <c r="B274">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>486</v>
+      </c>
+      <c r="B275">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>173</v>
+      </c>
+      <c r="B276">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>190</v>
+      </c>
+      <c r="B277">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>359</v>
+      </c>
+      <c r="B278">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>321</v>
+      </c>
+      <c r="B279">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>335</v>
+      </c>
+      <c r="B280">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>219</v>
+      </c>
+      <c r="B281">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>